<commit_message>
Updated the datasheets for the Longwave project.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28100" windowHeight="17560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,15 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Y [$/year]</t>
-  </si>
-  <si>
-    <t>w [$/year-worker]</t>
   </si>
   <si>
     <t>L [workers]</t>
@@ -38,22 +32,25 @@
     <t>N [capita]</t>
   </si>
   <si>
-    <t>b [births/year-capita]</t>
-  </si>
-  <si>
-    <t>d [deaths/year-capita]</t>
-  </si>
-  <si>
-    <t>m [migrations/year-capita]</t>
-  </si>
-  <si>
     <t>L_A [workers]</t>
   </si>
   <si>
     <t>E [GJ/year]</t>
   </si>
   <si>
-    <t>K [$]</t>
+    <t>Y [2005$/year]</t>
+  </si>
+  <si>
+    <t>w [2005$/year-worker]</t>
+  </si>
+  <si>
+    <t>D [deaths/year]</t>
+  </si>
+  <si>
+    <t>B [births/year]</t>
+  </si>
+  <si>
+    <t>K [2005$]</t>
   </si>
 </sst>
 </file>
@@ -121,7 +118,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,13 +126,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -445,1179 +443,1084 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J33"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1980</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>5833975000000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>39086</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>101400000</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>660939</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>227200000</v>
       </c>
-      <c r="G2" s="3">
-        <v>1.5899023000000002E-2</v>
-      </c>
-      <c r="H2" s="3">
-        <v>8.7581029999999997E-3</v>
+      <c r="G2" s="4">
+        <v>3612258</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1913841</v>
       </c>
       <c r="I2" s="3">
-        <v>3.104735E-3</v>
+        <v>7353330000000</v>
       </c>
       <c r="J2" s="4">
-        <v>7353330000000</v>
-      </c>
-      <c r="K2" s="5">
         <v>83112760950</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1981</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>5982075000000</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>39099</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>102500000</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>683300</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>229500000</v>
       </c>
-      <c r="G3" s="3">
-        <v>1.5813673E-2</v>
-      </c>
-      <c r="H3" s="3">
-        <v>8.6186539999999999E-3</v>
+      <c r="G3" s="4">
+        <v>3629238</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1989841</v>
       </c>
       <c r="I3" s="3">
-        <v>2.878397E-3</v>
+        <v>7590120000000</v>
       </c>
       <c r="J3" s="4">
-        <v>7590120000000</v>
-      </c>
-      <c r="K3" s="5">
         <v>81176408930</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1982</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>5865925000000</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>39125</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>101700000</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>711900</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>231700000</v>
       </c>
-      <c r="G4" s="3">
-        <v>1.5884925000000001E-2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>8.5230770000000004E-3</v>
+      <c r="G4" s="4">
+        <v>3680537</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1977981</v>
       </c>
       <c r="I4" s="3">
-        <v>2.8510670000000001E-3</v>
+        <v>7758610000000</v>
       </c>
       <c r="J4" s="4">
-        <v>7758610000000</v>
-      </c>
-      <c r="K4" s="5">
         <v>78029441540</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1983</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>6130925000000</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>39871</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>103000000</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>751700</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>233800000</v>
       </c>
-      <c r="G5" s="3">
-        <v>1.5564299E-2</v>
-      </c>
-      <c r="H5" s="3">
-        <v>8.6364460000000007E-3</v>
+      <c r="G5" s="4">
+        <v>3638933</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1974797</v>
       </c>
       <c r="I5" s="3">
-        <v>2.8254589999999998E-3</v>
+        <v>7963160000000</v>
       </c>
       <c r="J5" s="4">
-        <v>7963160000000</v>
-      </c>
-      <c r="K5" s="5">
         <v>77589648230</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1984</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>6571525000000</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>40421</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>107200000</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>797800</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>235800000</v>
       </c>
-      <c r="G6" s="3">
-        <v>1.5560394E-2</v>
-      </c>
-      <c r="H6" s="3">
-        <v>8.6487230000000005E-3</v>
+      <c r="G6" s="4">
+        <v>3669141</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2019201</v>
       </c>
       <c r="I6" s="3">
-        <v>2.8014939999999999E-3</v>
+        <v>8274440000000</v>
       </c>
       <c r="J6" s="4">
-        <v>8274440000000</v>
-      </c>
-      <c r="K6" s="5">
         <v>81427503780</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1985</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>6843400000000</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>41317</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>109400000</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>801900</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>237900000</v>
       </c>
-      <c r="G7" s="3">
-        <v>1.5807318000000001E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <v>8.7702400000000003E-3</v>
+      <c r="G7" s="4">
+        <v>3760561</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2039369</v>
       </c>
       <c r="I7" s="3">
-        <v>2.7767640000000001E-3</v>
+        <v>8616340000000</v>
       </c>
       <c r="J7" s="4">
-        <v>8616340000000</v>
-      </c>
-      <c r="K7" s="5">
         <v>81355952930</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1986</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>7080500000000</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>42421</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>111800000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>840381</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>240100000</v>
       </c>
-      <c r="G8" s="3">
-        <v>1.5645760000000002E-2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>8.7686840000000005E-3</v>
+      <c r="G8" s="4">
+        <v>3756547</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2086440</v>
       </c>
       <c r="I8" s="3">
-        <v>3.153861E-3</v>
+        <v>8950460000000</v>
       </c>
       <c r="J8" s="4">
-        <v>8950460000000</v>
-      </c>
-      <c r="K8" s="5">
         <v>81578376750</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1987</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>7307050000000</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>42911</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>114700000</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>895739</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>242300000</v>
       </c>
-      <c r="G9" s="3">
-        <v>1.5721808E-2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>8.7631989999999993E-3</v>
+      <c r="G9" s="4">
+        <v>3809394</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2105361</v>
       </c>
       <c r="I9" s="3">
-        <v>3.1252250000000001E-3</v>
+        <v>9271200000000</v>
       </c>
       <c r="J9" s="4">
-        <v>9271200000000</v>
-      </c>
-      <c r="K9" s="5">
         <v>84205348020</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1988</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>7607400000000</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>43349</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>117200000</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>900195</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>244500000</v>
       </c>
-      <c r="G10" s="3">
-        <v>1.5989816E-2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>8.8670720000000001E-3</v>
+      <c r="G10" s="4">
+        <v>3909510</v>
+      </c>
+      <c r="H10" s="6">
+        <v>2123323</v>
       </c>
       <c r="I10" s="3">
-        <v>3.0971039999999998E-3</v>
+        <v>9599010000000</v>
       </c>
       <c r="J10" s="4">
-        <v>9599010000000</v>
-      </c>
-      <c r="K10" s="5">
         <v>87997172270</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1989</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>7879175000000</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>44081</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>119600000</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>943036</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>246800000</v>
       </c>
-      <c r="G11" s="3">
-        <v>1.6373412E-2</v>
-      </c>
-      <c r="H11" s="3">
-        <v>8.7133950000000005E-3</v>
+      <c r="G11" s="4">
+        <v>4040958</v>
+      </c>
+      <c r="H11" s="6">
+        <v>2167999</v>
       </c>
       <c r="I11" s="3">
-        <v>3.0682410000000002E-3</v>
+        <v>9935250000000</v>
       </c>
       <c r="J11" s="4">
-        <v>9935250000000</v>
-      </c>
-      <c r="K11" s="5">
         <v>90695352450</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1990</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>8027025000000</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>43344</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>121000000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>960009</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>249600000</v>
       </c>
-      <c r="G12" s="3">
-        <v>1.6659502999999999E-2</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8.6076239999999995E-3</v>
+      <c r="G12" s="4">
+        <v>4158212</v>
+      </c>
+      <c r="H12" s="6">
+        <v>2150466</v>
       </c>
       <c r="I12" s="3">
-        <v>3.0338219999999998E-3</v>
+        <v>10241300000000</v>
       </c>
       <c r="J12" s="4">
-        <v>10241300000000</v>
-      </c>
-      <c r="K12" s="5">
         <v>91178022420</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1991</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>8008325000000</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>42726</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>119800000</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>981659</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>253000000</v>
       </c>
-      <c r="G13" s="3">
-        <v>1.6248644E-2</v>
-      </c>
-      <c r="H13" s="3">
-        <v>8.57517E-3</v>
+      <c r="G13" s="4">
+        <v>4110907</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2148463</v>
       </c>
       <c r="I13" s="3">
-        <v>3.5241909999999999E-3</v>
+        <v>10475400000000</v>
       </c>
       <c r="J13" s="4">
-        <v>10475400000000</v>
-      </c>
-      <c r="K13" s="5">
         <v>91154424090</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1992</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>8280025000000</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>43054</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>120500000</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>1020000</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>256500000</v>
       </c>
-      <c r="G14" s="3">
-        <v>1.5848008E-2</v>
-      </c>
-      <c r="H14" s="3">
-        <v>8.4819219999999994E-3</v>
+      <c r="G14" s="4">
+        <v>4065014</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2169518</v>
       </c>
       <c r="I14" s="3">
-        <v>3.4761029999999999E-3</v>
+        <v>10744600000000</v>
       </c>
       <c r="J14" s="4">
-        <v>10744600000000</v>
-      </c>
-      <c r="K14" s="5">
         <v>92448155690</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1993</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>8516175000000</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>44742</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>122100000</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>1014000</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>259900000</v>
       </c>
-      <c r="G15" s="3">
-        <v>1.5391458E-2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>8.7285609999999993E-3</v>
+      <c r="G15" s="4">
+        <v>4000240</v>
+      </c>
+      <c r="H15" s="6">
+        <v>2175613</v>
       </c>
       <c r="I15" s="3">
-        <v>3.4306290000000001E-3</v>
+        <v>11065300000000</v>
       </c>
       <c r="J15" s="4">
-        <v>11065300000000</v>
-      </c>
-      <c r="K15" s="5">
         <v>94232721890</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1994</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>8863125000000</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>45380</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>124800000</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>1080000</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>263100000</v>
       </c>
-      <c r="G16" s="3">
-        <v>1.502382E-2</v>
-      </c>
-      <c r="H16" s="3">
-        <v>8.6620829999999992E-3</v>
+      <c r="G16" s="4">
+        <v>3952767</v>
+      </c>
+      <c r="H16" s="6">
+        <v>2268553</v>
       </c>
       <c r="I16" s="3">
-        <v>3.388903E-3</v>
+        <v>11449300000000</v>
       </c>
       <c r="J16" s="4">
-        <v>11449300000000</v>
-      </c>
-      <c r="K16" s="5">
         <v>96065748930</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1995</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>9085975000000</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>45859</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>126500000</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>1036000</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>266300000</v>
       </c>
-      <c r="G17" s="3">
-        <v>1.4643593999999999E-2</v>
-      </c>
-      <c r="H17" s="3">
-        <v>8.6824329999999998E-3</v>
+      <c r="G17" s="4">
+        <v>3899589</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2278994</v>
       </c>
       <c r="I17" s="3">
-        <v>3.3481800000000001E-3</v>
+        <v>11879000000000</v>
       </c>
       <c r="J17" s="4">
-        <v>11879000000000</v>
-      </c>
-      <c r="K17" s="5">
         <v>98186495330</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1996</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>9425850000000</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>46823</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>128300000</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>1139000</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>269400000</v>
       </c>
-      <c r="G18" s="3">
-        <v>1.4445041E-2</v>
-      </c>
-      <c r="H18" s="3">
-        <v>8.5920189999999994E-3</v>
+      <c r="G18" s="4">
+        <v>3891494</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2312132</v>
       </c>
       <c r="I18" s="3">
-        <v>6.3262489999999999E-3</v>
+        <v>12389100000000</v>
       </c>
       <c r="J18" s="4">
-        <v>12389100000000</v>
-      </c>
-      <c r="K18" s="5">
         <v>101378213900</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1997</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>9845925000000</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>47995</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>131100000</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>1160000</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>272700000</v>
       </c>
-      <c r="G19" s="3">
-        <v>1.4231367999999999E-2</v>
-      </c>
-      <c r="H19" s="3">
-        <v>8.4864139999999994E-3</v>
+      <c r="G19" s="4">
+        <v>3880894</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2314690</v>
       </c>
       <c r="I19" s="3">
-        <v>6.2496940000000001E-3</v>
+        <v>12987200000000</v>
       </c>
       <c r="J19" s="4">
-        <v>12987200000000</v>
-      </c>
-      <c r="K19" s="5">
         <v>102230767700</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1998</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>10274750000000</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>49276</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>133000000</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>1199000</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>275900000</v>
       </c>
-      <c r="G20" s="3">
-        <v>1.4286165E-2</v>
-      </c>
-      <c r="H20" s="3">
-        <v>8.4713879999999998E-3</v>
+      <c r="G20" s="4">
+        <v>3941553</v>
+      </c>
+      <c r="H20" s="6">
+        <v>2314245</v>
       </c>
       <c r="I20" s="3">
-        <v>6.177208E-3</v>
+        <v>13702500000000</v>
       </c>
       <c r="J20" s="4">
-        <v>13702500000000</v>
-      </c>
-      <c r="K20" s="5">
         <v>102919340800</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1999</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>10770630000000</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>51136</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>134900000</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>1261000</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>279000000</v>
       </c>
-      <c r="G21" s="3">
-        <v>1.4191459E-2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>8.5713230000000005E-3</v>
+      <c r="G21" s="4">
+        <v>3959417</v>
+      </c>
+      <c r="H21" s="6">
+        <v>2337256</v>
       </c>
       <c r="I21" s="3">
-        <v>6.1085719999999996E-3</v>
+        <v>14518800000000</v>
       </c>
       <c r="J21" s="4">
-        <v>14518800000000</v>
-      </c>
-      <c r="K21" s="5">
         <v>104583817300</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2000</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>11216430000000</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>51388</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>138300000</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>1294000</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>282200000</v>
       </c>
-      <c r="G22" s="3">
-        <v>1.4382756999999999E-2</v>
-      </c>
-      <c r="H22" s="3">
-        <v>8.5164809999999994E-3</v>
+      <c r="G22" s="4">
+        <v>4058814</v>
+      </c>
+      <c r="H22" s="6">
+        <v>2391399</v>
       </c>
       <c r="I22" s="3">
-        <v>6.0393039999999997E-3</v>
+        <v>15409200000000</v>
       </c>
       <c r="J22" s="4">
-        <v>15409200000000</v>
-      </c>
-      <c r="K22" s="5">
         <v>106936290200</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2001</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>11337480000000</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>51478</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>138400000</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>1320000</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>285000000</v>
       </c>
-      <c r="G23" s="3">
-        <v>1.4126081E-2</v>
-      </c>
-      <c r="H23" s="3">
-        <v>8.4786840000000002E-3</v>
+      <c r="G23" s="4">
+        <v>4025933</v>
+      </c>
+      <c r="H23" s="6">
+        <v>2403351</v>
       </c>
       <c r="I23" s="3">
-        <v>4.3475069999999996E-3</v>
+        <v>16201300000000</v>
       </c>
       <c r="J23" s="4">
-        <v>16201300000000</v>
-      </c>
-      <c r="K23" s="5">
         <v>104444769100</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2002</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>11543100000000</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>51193</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>138000000</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>1342000</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>287600000</v>
       </c>
-      <c r="G24" s="3">
-        <v>1.3983748000000001E-2</v>
-      </c>
-      <c r="H24" s="3">
-        <v>8.4957820000000003E-3</v>
+      <c r="G24" s="4">
+        <v>4021726</v>
+      </c>
+      <c r="H24" s="6">
+        <v>2416425</v>
       </c>
       <c r="I24" s="3">
-        <v>4.3082040000000004E-3</v>
+        <v>16858700000000</v>
       </c>
       <c r="J24" s="4">
-        <v>16858700000000</v>
-      </c>
-      <c r="K24" s="5">
         <v>106391985300</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2003</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>11836430000000</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>51181</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>139400000</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>1431000</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>290100000</v>
       </c>
-      <c r="G25" s="3">
-        <v>1.4098414E-2</v>
-      </c>
-      <c r="H25" s="3">
-        <v>8.439462E-3</v>
+      <c r="G25" s="4">
+        <v>4089950</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2443387</v>
       </c>
       <c r="I25" s="3">
-        <v>4.2710769999999999E-3</v>
+        <v>17533300000000</v>
       </c>
       <c r="J25" s="4">
-        <v>17533300000000</v>
-      </c>
-      <c r="K25" s="5">
         <v>106687896600</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2004</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>12246930000000</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>51109</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>140900000</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>1385000</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>292800000</v>
       </c>
-      <c r="G26" s="3">
-        <v>1.4043893E-2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>8.1885759999999995E-3</v>
+      <c r="G26" s="4">
+        <v>4112052</v>
+      </c>
+      <c r="H26" s="6">
+        <v>2448288</v>
       </c>
       <c r="I26" s="3">
-        <v>4.2316919999999996E-3</v>
+        <v>18298400000000</v>
       </c>
       <c r="J26" s="4">
-        <v>18298400000000</v>
-      </c>
-      <c r="K26" s="5">
         <v>108508357500</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2005</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>12622950000000</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>52292</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>143400000</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>1375000</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>295500000</v>
       </c>
-      <c r="G27" s="3">
-        <v>1.4004565E-2</v>
-      </c>
-      <c r="H27" s="3">
-        <v>8.2843210000000007E-3</v>
+      <c r="G27" s="4">
+        <v>4138349</v>
+      </c>
+      <c r="H27" s="6">
+        <v>2397615</v>
       </c>
       <c r="I27" s="3">
-        <v>4.1930270000000002E-3</v>
+        <v>19139900000000</v>
       </c>
       <c r="J27" s="4">
-        <v>19139900000000</v>
-      </c>
-      <c r="K27" s="5">
         <v>108705755300</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2006</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>12958480000000</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>53620</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>146000000</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>1414000</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <v>298400000</v>
       </c>
-      <c r="G28" s="3">
-        <v>1.4294754999999999E-2</v>
-      </c>
-      <c r="H28" s="3">
-        <v>8.1309120000000006E-3</v>
+      <c r="G28" s="4">
+        <v>4265555</v>
+      </c>
+      <c r="H28" s="6">
+        <v>2448017</v>
       </c>
       <c r="I28" s="3">
-        <v>3.3209950000000002E-3</v>
+        <v>19972800000000</v>
       </c>
       <c r="J28" s="4">
-        <v>19972800000000</v>
-      </c>
-      <c r="K28" s="5">
         <v>108223082400</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2007</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>13206380000000</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>53434</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>147600000</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>1413000</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <v>301200000</v>
       </c>
-      <c r="G29" s="3">
-        <v>1.4330123E-2</v>
-      </c>
-      <c r="H29" s="3">
-        <v>8.0468529999999996E-3</v>
+      <c r="G29" s="4">
+        <v>4316233</v>
+      </c>
+      <c r="H29" s="6">
+        <v>2426264</v>
       </c>
       <c r="I29" s="3">
-        <v>3.2901219999999999E-3</v>
+        <v>20705300000000</v>
       </c>
       <c r="J29" s="4">
-        <v>20705300000000</v>
-      </c>
-      <c r="K29" s="5">
         <v>110168847900</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2008</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>13161930000000</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>51503</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>147000000</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>1498000</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>304100000</v>
       </c>
-      <c r="G30" s="3">
-        <v>1.3968082999999999E-2</v>
-      </c>
-      <c r="H30" s="3">
-        <v>8.1288520000000006E-3</v>
+      <c r="G30" s="4">
+        <v>4247694</v>
+      </c>
+      <c r="H30" s="6">
+        <v>2423712</v>
       </c>
       <c r="I30" s="3">
-        <v>3.2587459999999999E-3</v>
+        <v>21234600000000</v>
       </c>
       <c r="J30" s="4">
-        <v>21234600000000</v>
-      </c>
-      <c r="K30" s="5">
         <v>107871770000</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2009</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>12703130000000</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>50410</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>141500000</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>1528000</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>306800000</v>
       </c>
-      <c r="G31" s="3">
-        <v>1.3463706000000001E-2</v>
-      </c>
-      <c r="H31" s="3">
-        <v>7.9438170000000006E-3</v>
+      <c r="G31" s="4">
+        <v>4130665</v>
+      </c>
+      <c r="H31" s="6">
+        <v>2471984</v>
       </c>
       <c r="I31" s="3">
-        <v>3.230068E-3</v>
+        <v>21354500000000</v>
       </c>
       <c r="J31" s="4">
-        <v>21354500000000</v>
-      </c>
-      <c r="K31" s="5">
         <v>103272113700</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2010</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>13087980000000</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>49692</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>140700000</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>1558000</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>309300000</v>
       </c>
-      <c r="G32" s="3">
-        <v>1.2930443E-2</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7.9807149999999993E-3</v>
+      <c r="G32" s="4">
+        <v>3999386</v>
+      </c>
+      <c r="H32" s="6">
+        <v>2437163</v>
       </c>
       <c r="I32" s="3">
-        <v>3.2039600000000001E-3</v>
+        <v>21508000000000</v>
       </c>
       <c r="J32" s="4">
-        <v>21508000000000</v>
-      </c>
-      <c r="K32" s="5">
         <v>107139605300</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2011</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>13315080000000</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>50124</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>141500000</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>1588000</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>311600000</v>
       </c>
-      <c r="G33" s="3">
-        <v>1.2688039E-2</v>
-      </c>
-      <c r="H33" s="3">
-        <v>8.0653789999999993E-3</v>
+      <c r="G33" s="4">
+        <v>3953593</v>
+      </c>
+      <c r="H33" s="5">
+        <v>2468435</v>
       </c>
       <c r="I33" s="3">
-        <v>3.1803109999999999E-3</v>
+        <v>21763500000000</v>
       </c>
       <c r="J33" s="4">
-        <v>21763500000000</v>
-      </c>
-      <c r="K33" s="5">
         <v>106735322000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="6">
+        <v>2513172</v>
       </c>
     </row>
   </sheetData>
@@ -1637,7 +1540,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1654,7 +1557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added comments to the top of the USData.xlsx file to make units clear.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21780" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,36 +21,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>L [workers]</t>
-  </si>
-  <si>
-    <t>N [capita]</t>
-  </si>
-  <si>
-    <t>L_A [workers]</t>
-  </si>
-  <si>
-    <t>E [GJ/year]</t>
-  </si>
-  <si>
-    <t>Y [2005$/year]</t>
-  </si>
-  <si>
-    <t>w [2005$/year-worker]</t>
-  </si>
-  <si>
-    <t>D [deaths/year]</t>
-  </si>
-  <si>
-    <t>B [births/year]</t>
-  </si>
-  <si>
-    <t>K [2005$]</t>
+    <t># N = total U.S. population [capita]</t>
+  </si>
+  <si>
+    <t># B = births in the U.S. [births/year]</t>
+  </si>
+  <si>
+    <t># D = deaths in the U.S. [deaths/year]</t>
+  </si>
+  <si>
+    <t># L_A = total number of U.S. researchers in the STEM disciplines [workers/year]</t>
+  </si>
+  <si>
+    <t># L = U.S. labor [workers/year]</t>
+  </si>
+  <si>
+    <t># Y = U.S. GDP [2005$/year]</t>
+  </si>
+  <si>
+    <t># w = Average U.S. wage [2005$/year-worker]</t>
+  </si>
+  <si>
+    <t># K = U.S. capital stock [2005$]</t>
+  </si>
+  <si>
+    <t># E = U.S. thermal energy consumption [GJ/year]</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L_A</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -443,1085 +473,1133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2">
         <v>1980</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B12" s="3">
         <v>5833975000000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C12" s="3">
         <v>39086</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D12" s="3">
         <v>101400000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E12" s="3">
         <v>660939</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F12" s="3">
         <v>227200000</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G12" s="4">
         <v>3612258</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H12" s="6">
         <v>1913841</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I12" s="3">
         <v>7353330000000</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J12" s="4">
         <v>83112760950</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="13" spans="1:10">
+      <c r="A13" s="2">
         <v>1981</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B13" s="3">
         <v>5982075000000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C13" s="3">
         <v>39099</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D13" s="3">
         <v>102500000</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E13" s="3">
         <v>683300</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F13" s="3">
         <v>229500000</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G13" s="4">
         <v>3629238</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H13" s="6">
         <v>1989841</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I13" s="3">
         <v>7590120000000</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J13" s="4">
         <v>81176408930</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="14" spans="1:10">
+      <c r="A14" s="2">
         <v>1982</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B14" s="3">
         <v>5865925000000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C14" s="3">
         <v>39125</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D14" s="3">
         <v>101700000</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E14" s="3">
         <v>711900</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F14" s="3">
         <v>231700000</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G14" s="4">
         <v>3680537</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H14" s="6">
         <v>1977981</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I14" s="3">
         <v>7758610000000</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J14" s="4">
         <v>78029441540</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="15" spans="1:10">
+      <c r="A15" s="2">
         <v>1983</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B15" s="3">
         <v>6130925000000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C15" s="3">
         <v>39871</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D15" s="3">
         <v>103000000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E15" s="3">
         <v>751700</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F15" s="3">
         <v>233800000</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G15" s="4">
         <v>3638933</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H15" s="6">
         <v>1974797</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I15" s="3">
         <v>7963160000000</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J15" s="4">
         <v>77589648230</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="16" spans="1:10">
+      <c r="A16" s="2">
         <v>1984</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B16" s="3">
         <v>6571525000000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C16" s="3">
         <v>40421</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D16" s="3">
         <v>107200000</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E16" s="3">
         <v>797800</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F16" s="3">
         <v>235800000</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G16" s="4">
         <v>3669141</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H16" s="6">
         <v>2019201</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I16" s="3">
         <v>8274440000000</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J16" s="4">
         <v>81427503780</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="17" spans="1:10">
+      <c r="A17" s="2">
         <v>1985</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B17" s="3">
         <v>6843400000000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C17" s="3">
         <v>41317</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D17" s="3">
         <v>109400000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E17" s="3">
         <v>801900</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F17" s="3">
         <v>237900000</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G17" s="4">
         <v>3760561</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H17" s="6">
         <v>2039369</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I17" s="3">
         <v>8616340000000</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J17" s="4">
         <v>81355952930</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="18" spans="1:10">
+      <c r="A18" s="2">
         <v>1986</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B18" s="3">
         <v>7080500000000</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C18" s="3">
         <v>42421</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D18" s="3">
         <v>111800000</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E18" s="3">
         <v>840381</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F18" s="3">
         <v>240100000</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G18" s="4">
         <v>3756547</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H18" s="6">
         <v>2086440</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I18" s="3">
         <v>8950460000000</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J18" s="4">
         <v>81578376750</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="19" spans="1:10">
+      <c r="A19" s="2">
         <v>1987</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B19" s="3">
         <v>7307050000000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C19" s="3">
         <v>42911</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D19" s="3">
         <v>114700000</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E19" s="3">
         <v>895739</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F19" s="3">
         <v>242300000</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G19" s="4">
         <v>3809394</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H19" s="6">
         <v>2105361</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I19" s="3">
         <v>9271200000000</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J19" s="4">
         <v>84205348020</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="20" spans="1:10">
+      <c r="A20" s="2">
         <v>1988</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B20" s="3">
         <v>7607400000000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C20" s="3">
         <v>43349</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D20" s="3">
         <v>117200000</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E20" s="3">
         <v>900195</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F20" s="3">
         <v>244500000</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G20" s="4">
         <v>3909510</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H20" s="6">
         <v>2123323</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I20" s="3">
         <v>9599010000000</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J20" s="4">
         <v>87997172270</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="21" spans="1:10">
+      <c r="A21" s="2">
         <v>1989</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B21" s="3">
         <v>7879175000000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C21" s="3">
         <v>44081</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D21" s="3">
         <v>119600000</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E21" s="3">
         <v>943036</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F21" s="3">
         <v>246800000</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G21" s="4">
         <v>4040958</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H21" s="6">
         <v>2167999</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I21" s="3">
         <v>9935250000000</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J21" s="4">
         <v>90695352450</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="22" spans="1:10">
+      <c r="A22" s="2">
         <v>1990</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B22" s="3">
         <v>8027025000000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C22" s="3">
         <v>43344</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D22" s="3">
         <v>121000000</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E22" s="3">
         <v>960009</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F22" s="3">
         <v>249600000</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G22" s="4">
         <v>4158212</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H22" s="6">
         <v>2150466</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I22" s="3">
         <v>10241300000000</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J22" s="4">
         <v>91178022420</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="23" spans="1:10">
+      <c r="A23" s="2">
         <v>1991</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B23" s="3">
         <v>8008325000000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C23" s="3">
         <v>42726</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D23" s="3">
         <v>119800000</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E23" s="3">
         <v>981659</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F23" s="3">
         <v>253000000</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G23" s="4">
         <v>4110907</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H23" s="6">
         <v>2148463</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I23" s="3">
         <v>10475400000000</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J23" s="4">
         <v>91154424090</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="24" spans="1:10">
+      <c r="A24" s="2">
         <v>1992</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B24" s="3">
         <v>8280025000000</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C24" s="3">
         <v>43054</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D24" s="3">
         <v>120500000</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E24" s="3">
         <v>1020000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F24" s="3">
         <v>256500000</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G24" s="4">
         <v>4065014</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H24" s="6">
         <v>2169518</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I24" s="3">
         <v>10744600000000</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J24" s="4">
         <v>92448155690</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="25" spans="1:10">
+      <c r="A25" s="2">
         <v>1993</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B25" s="3">
         <v>8516175000000</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C25" s="3">
         <v>44742</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D25" s="3">
         <v>122100000</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E25" s="3">
         <v>1014000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F25" s="3">
         <v>259900000</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G25" s="4">
         <v>4000240</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H25" s="6">
         <v>2175613</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I25" s="3">
         <v>11065300000000</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J25" s="4">
         <v>94232721890</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="26" spans="1:10">
+      <c r="A26" s="2">
         <v>1994</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B26" s="3">
         <v>8863125000000</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C26" s="3">
         <v>45380</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D26" s="3">
         <v>124800000</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E26" s="3">
         <v>1080000</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F26" s="3">
         <v>263100000</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G26" s="4">
         <v>3952767</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H26" s="6">
         <v>2268553</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I26" s="3">
         <v>11449300000000</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J26" s="4">
         <v>96065748930</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="27" spans="1:10">
+      <c r="A27" s="2">
         <v>1995</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B27" s="3">
         <v>9085975000000</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C27" s="3">
         <v>45859</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D27" s="3">
         <v>126500000</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E27" s="3">
         <v>1036000</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F27" s="3">
         <v>266300000</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G27" s="4">
         <v>3899589</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H27" s="6">
         <v>2278994</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I27" s="3">
         <v>11879000000000</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J27" s="4">
         <v>98186495330</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="28" spans="1:10">
+      <c r="A28" s="2">
         <v>1996</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B28" s="3">
         <v>9425850000000</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C28" s="3">
         <v>46823</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D28" s="3">
         <v>128300000</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E28" s="3">
         <v>1139000</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F28" s="3">
         <v>269400000</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G28" s="4">
         <v>3891494</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H28" s="6">
         <v>2312132</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I28" s="3">
         <v>12389100000000</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J28" s="4">
         <v>101378213900</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="29" spans="1:10">
+      <c r="A29" s="2">
         <v>1997</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B29" s="3">
         <v>9845925000000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C29" s="3">
         <v>47995</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D29" s="3">
         <v>131100000</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E29" s="3">
         <v>1160000</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F29" s="3">
         <v>272700000</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G29" s="4">
         <v>3880894</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H29" s="6">
         <v>2314690</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I29" s="3">
         <v>12987200000000</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J29" s="4">
         <v>102230767700</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="30" spans="1:10">
+      <c r="A30" s="2">
         <v>1998</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B30" s="3">
         <v>10274750000000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C30" s="3">
         <v>49276</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D30" s="3">
         <v>133000000</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E30" s="3">
         <v>1199000</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F30" s="3">
         <v>275900000</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G30" s="4">
         <v>3941553</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H30" s="6">
         <v>2314245</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I30" s="3">
         <v>13702500000000</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J30" s="4">
         <v>102919340800</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="31" spans="1:10">
+      <c r="A31" s="2">
         <v>1999</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B31" s="3">
         <v>10770630000000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C31" s="3">
         <v>51136</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D31" s="3">
         <v>134900000</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E31" s="3">
         <v>1261000</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F31" s="3">
         <v>279000000</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G31" s="4">
         <v>3959417</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H31" s="6">
         <v>2337256</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I31" s="3">
         <v>14518800000000</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J31" s="4">
         <v>104583817300</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="32" spans="1:10">
+      <c r="A32" s="2">
         <v>2000</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B32" s="3">
         <v>11216430000000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C32" s="3">
         <v>51388</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D32" s="3">
         <v>138300000</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E32" s="3">
         <v>1294000</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F32" s="3">
         <v>282200000</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G32" s="4">
         <v>4058814</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H32" s="6">
         <v>2391399</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I32" s="3">
         <v>15409200000000</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J32" s="4">
         <v>106936290200</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="33" spans="1:10">
+      <c r="A33" s="2">
         <v>2001</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B33" s="3">
         <v>11337480000000</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C33" s="3">
         <v>51478</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D33" s="3">
         <v>138400000</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E33" s="3">
         <v>1320000</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F33" s="3">
         <v>285000000</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G33" s="4">
         <v>4025933</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H33" s="6">
         <v>2403351</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I33" s="3">
         <v>16201300000000</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J33" s="4">
         <v>104444769100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="34" spans="1:10">
+      <c r="A34" s="2">
         <v>2002</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B34" s="3">
         <v>11543100000000</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C34" s="3">
         <v>51193</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D34" s="3">
         <v>138000000</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E34" s="3">
         <v>1342000</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F34" s="3">
         <v>287600000</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G34" s="4">
         <v>4021726</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H34" s="6">
         <v>2416425</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I34" s="3">
         <v>16858700000000</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J34" s="4">
         <v>106391985300</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="35" spans="1:10">
+      <c r="A35" s="2">
         <v>2003</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B35" s="3">
         <v>11836430000000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C35" s="3">
         <v>51181</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D35" s="3">
         <v>139400000</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E35" s="3">
         <v>1431000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F35" s="3">
         <v>290100000</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G35" s="4">
         <v>4089950</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H35" s="6">
         <v>2443387</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I35" s="3">
         <v>17533300000000</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J35" s="4">
         <v>106687896600</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="36" spans="1:10">
+      <c r="A36" s="2">
         <v>2004</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B36" s="3">
         <v>12246930000000</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C36" s="3">
         <v>51109</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D36" s="3">
         <v>140900000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E36" s="3">
         <v>1385000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F36" s="3">
         <v>292800000</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G36" s="4">
         <v>4112052</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H36" s="6">
         <v>2448288</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I36" s="3">
         <v>18298400000000</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J36" s="4">
         <v>108508357500</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="37" spans="1:10">
+      <c r="A37" s="2">
         <v>2005</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B37" s="3">
         <v>12622950000000</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C37" s="3">
         <v>52292</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D37" s="3">
         <v>143400000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E37" s="3">
         <v>1375000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F37" s="3">
         <v>295500000</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G37" s="4">
         <v>4138349</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H37" s="6">
         <v>2397615</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I37" s="3">
         <v>19139900000000</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J37" s="4">
         <v>108705755300</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="38" spans="1:10">
+      <c r="A38" s="2">
         <v>2006</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B38" s="3">
         <v>12958480000000</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C38" s="3">
         <v>53620</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D38" s="3">
         <v>146000000</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E38" s="3">
         <v>1414000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F38" s="3">
         <v>298400000</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G38" s="4">
         <v>4265555</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H38" s="6">
         <v>2448017</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I38" s="3">
         <v>19972800000000</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J38" s="4">
         <v>108223082400</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="39" spans="1:10">
+      <c r="A39" s="2">
         <v>2007</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B39" s="3">
         <v>13206380000000</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C39" s="3">
         <v>53434</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D39" s="3">
         <v>147600000</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E39" s="3">
         <v>1413000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F39" s="3">
         <v>301200000</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G39" s="4">
         <v>4316233</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H39" s="6">
         <v>2426264</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I39" s="3">
         <v>20705300000000</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J39" s="4">
         <v>110168847900</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="40" spans="1:10">
+      <c r="A40" s="2">
         <v>2008</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B40" s="3">
         <v>13161930000000</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C40" s="3">
         <v>51503</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D40" s="3">
         <v>147000000</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E40" s="3">
         <v>1498000</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F40" s="3">
         <v>304100000</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G40" s="4">
         <v>4247694</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H40" s="6">
         <v>2423712</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I40" s="3">
         <v>21234600000000</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J40" s="4">
         <v>107871770000</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="41" spans="1:10">
+      <c r="A41" s="2">
         <v>2009</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B41" s="3">
         <v>12703130000000</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C41" s="3">
         <v>50410</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D41" s="3">
         <v>141500000</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E41" s="3">
         <v>1528000</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F41" s="3">
         <v>306800000</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G41" s="4">
         <v>4130665</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H41" s="6">
         <v>2471984</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I41" s="3">
         <v>21354500000000</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J41" s="4">
         <v>103272113700</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="42" spans="1:10">
+      <c r="A42" s="2">
         <v>2010</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B42" s="3">
         <v>13087980000000</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C42" s="3">
         <v>49692</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D42" s="3">
         <v>140700000</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E42" s="3">
         <v>1558000</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F42" s="3">
         <v>309300000</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G42" s="4">
         <v>3999386</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H42" s="6">
         <v>2437163</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I42" s="3">
         <v>21508000000000</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J42" s="4">
         <v>107139605300</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="43" spans="1:10">
+      <c r="A43" s="2">
         <v>2011</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B43" s="3">
         <v>13315080000000</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C43" s="3">
         <v>50124</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D43" s="3">
         <v>141500000</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E43" s="3">
         <v>1588000</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F43" s="3">
         <v>311600000</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G43" s="4">
         <v>3953593</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H43" s="5">
         <v>2468435</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I43" s="3">
         <v>21763500000000</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J43" s="4">
         <v>106735322000</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H34" s="6">
-        <v>2513172</v>
-      </c>
+    <row r="44" spans="1:10">
+      <c r="H44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1540,7 +1618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1557,7 +1635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Edited the comment on wages to indicate that wages in the raw data file are in 2005$/year-capita, not 2005$/year-worker.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -44,9 +44,6 @@
     <t># Y = U.S. GDP [2005$/year]</t>
   </si>
   <si>
-    <t># w = Average U.S. wage [2005$/year-worker]</t>
-  </si>
-  <si>
     <t># K = U.S. capital stock [2005$]</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t># w = Average U.S. wage [2005$/year-capita]</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -499,7 +499,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -529,17 +529,17 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -547,31 +547,31 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:10">

</xml_diff>

<commit_message>
Changed name of wage column to w_capita to indicate that it is wages per capita.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -35,12 +33,6 @@
     <t># D = deaths in the U.S. [deaths/year]</t>
   </si>
   <si>
-    <t># L_A = total number of U.S. researchers in the STEM disciplines [workers/year]</t>
-  </si>
-  <si>
-    <t># L = U.S. labor [workers/year]</t>
-  </si>
-  <si>
     <t># Y = U.S. GDP [2005$/year]</t>
   </si>
   <si>
@@ -56,9 +48,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -80,7 +69,16 @@
     <t>E</t>
   </si>
   <si>
-    <t># w = Average U.S. wage [2005$/year-capita]</t>
+    <t>w_capita</t>
+  </si>
+  <si>
+    <t># w_capita = Average U.S. wage [2005$/year-capita]</t>
+  </si>
+  <si>
+    <t># L =total U.S. labor [workers/year]</t>
+  </si>
+  <si>
+    <t># L_A = number of U.S. researchers in the STEM disciplines [workers/year]</t>
   </si>
 </sst>
 </file>
@@ -476,7 +474,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -494,22 +492,22 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -529,17 +527,17 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -547,31 +545,31 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1610,38 +1608,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Now correctly noting that the wage data in the file is wages per capita.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -146,21 +146,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -471,11 +466,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -576,31 +569,31 @@
       <c r="A12" s="2">
         <v>1980</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>5833975000000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>39086</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>101400000</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>660939</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>227200000</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="2">
         <v>3612258</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="3">
         <v>1913841</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>7353330000000</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="2">
         <v>83112760950</v>
       </c>
     </row>
@@ -608,31 +601,31 @@
       <c r="A13" s="2">
         <v>1981</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>5982075000000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>39099</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>102500000</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>683300</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>229500000</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <v>3629238</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="3">
         <v>1989841</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>7590120000000</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="2">
         <v>81176408930</v>
       </c>
     </row>
@@ -640,31 +633,31 @@
       <c r="A14" s="2">
         <v>1982</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>5865925000000</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>39125</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>101700000</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>711900</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>231700000</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="2">
         <v>3680537</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="3">
         <v>1977981</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>7758610000000</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="2">
         <v>78029441540</v>
       </c>
     </row>
@@ -672,31 +665,31 @@
       <c r="A15" s="2">
         <v>1983</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>6130925000000</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>39871</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>103000000</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>751700</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>233800000</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="2">
         <v>3638933</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="3">
         <v>1974797</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>7963160000000</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="2">
         <v>77589648230</v>
       </c>
     </row>
@@ -704,31 +697,31 @@
       <c r="A16" s="2">
         <v>1984</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>6571525000000</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>40421</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>107200000</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>797800</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>235800000</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="2">
         <v>3669141</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="3">
         <v>2019201</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>8274440000000</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="2">
         <v>81427503780</v>
       </c>
     </row>
@@ -736,31 +729,31 @@
       <c r="A17" s="2">
         <v>1985</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>6843400000000</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>41317</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>109400000</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>801900</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>237900000</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <v>3760561</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="3">
         <v>2039369</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>8616340000000</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="2">
         <v>81355952930</v>
       </c>
     </row>
@@ -768,31 +761,31 @@
       <c r="A18" s="2">
         <v>1986</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>7080500000000</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>42421</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>111800000</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>840381</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>240100000</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <v>3756547</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="3">
         <v>2086440</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>8950460000000</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="2">
         <v>81578376750</v>
       </c>
     </row>
@@ -800,31 +793,31 @@
       <c r="A19" s="2">
         <v>1987</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>7307050000000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>42911</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>114700000</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>895739</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>242300000</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="2">
         <v>3809394</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="3">
         <v>2105361</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>9271200000000</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="2">
         <v>84205348020</v>
       </c>
     </row>
@@ -832,31 +825,31 @@
       <c r="A20" s="2">
         <v>1988</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>7607400000000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>43349</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>117200000</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>900195</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>244500000</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <v>3909510</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="3">
         <v>2123323</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>9599010000000</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="2">
         <v>87997172270</v>
       </c>
     </row>
@@ -864,31 +857,31 @@
       <c r="A21" s="2">
         <v>1989</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>7879175000000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>44081</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>119600000</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>943036</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>246800000</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="2">
         <v>4040958</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="3">
         <v>2167999</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>9935250000000</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="2">
         <v>90695352450</v>
       </c>
     </row>
@@ -896,31 +889,31 @@
       <c r="A22" s="2">
         <v>1990</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>8027025000000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>43344</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>121000000</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>960009</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>249600000</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="2">
         <v>4158212</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="3">
         <v>2150466</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>10241300000000</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="2">
         <v>91178022420</v>
       </c>
     </row>
@@ -928,31 +921,31 @@
       <c r="A23" s="2">
         <v>1991</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>8008325000000</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>42726</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>119800000</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>981659</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>253000000</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>4110907</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="3">
         <v>2148463</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>10475400000000</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="2">
         <v>91154424090</v>
       </c>
     </row>
@@ -960,31 +953,31 @@
       <c r="A24" s="2">
         <v>1992</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>8280025000000</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>43054</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>120500000</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>1020000</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>256500000</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="2">
         <v>4065014</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="3">
         <v>2169518</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>10744600000000</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="2">
         <v>92448155690</v>
       </c>
     </row>
@@ -992,31 +985,31 @@
       <c r="A25" s="2">
         <v>1993</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>8516175000000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>44742</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>122100000</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>1014000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>259900000</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="2">
         <v>4000240</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="3">
         <v>2175613</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>11065300000000</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="2">
         <v>94232721890</v>
       </c>
     </row>
@@ -1024,31 +1017,31 @@
       <c r="A26" s="2">
         <v>1994</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>8863125000000</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>45380</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>124800000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>1080000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>263100000</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="2">
         <v>3952767</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="3">
         <v>2268553</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <v>11449300000000</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="2">
         <v>96065748930</v>
       </c>
     </row>
@@ -1056,31 +1049,31 @@
       <c r="A27" s="2">
         <v>1995</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>9085975000000</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>45859</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>126500000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1036000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>266300000</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="2">
         <v>3899589</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="3">
         <v>2278994</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>11879000000000</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="2">
         <v>98186495330</v>
       </c>
     </row>
@@ -1088,31 +1081,31 @@
       <c r="A28" s="2">
         <v>1996</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>9425850000000</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>46823</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>128300000</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>1139000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>269400000</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="2">
         <v>3891494</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="3">
         <v>2312132</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>12389100000000</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="2">
         <v>101378213900</v>
       </c>
     </row>
@@ -1120,31 +1113,31 @@
       <c r="A29" s="2">
         <v>1997</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>9845925000000</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>47995</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>131100000</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1160000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>272700000</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="2">
         <v>3880894</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="3">
         <v>2314690</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <v>12987200000000</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="2">
         <v>102230767700</v>
       </c>
     </row>
@@ -1152,31 +1145,31 @@
       <c r="A30" s="2">
         <v>1998</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>10274750000000</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>49276</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>133000000</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1199000</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>275900000</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="2">
         <v>3941553</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="3">
         <v>2314245</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>13702500000000</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="2">
         <v>102919340800</v>
       </c>
     </row>
@@ -1184,31 +1177,31 @@
       <c r="A31" s="2">
         <v>1999</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>10770630000000</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>51136</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>134900000</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>1261000</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>279000000</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="2">
         <v>3959417</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="3">
         <v>2337256</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>14518800000000</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="2">
         <v>104583817300</v>
       </c>
     </row>
@@ -1216,31 +1209,31 @@
       <c r="A32" s="2">
         <v>2000</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>11216430000000</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>51388</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>138300000</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>1294000</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>282200000</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="2">
         <v>4058814</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="3">
         <v>2391399</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>15409200000000</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="2">
         <v>106936290200</v>
       </c>
     </row>
@@ -1248,31 +1241,31 @@
       <c r="A33" s="2">
         <v>2001</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>11337480000000</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>51478</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>138400000</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>1320000</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>285000000</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="2">
         <v>4025933</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="3">
         <v>2403351</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="2">
         <v>16201300000000</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="2">
         <v>104444769100</v>
       </c>
     </row>
@@ -1280,31 +1273,31 @@
       <c r="A34" s="2">
         <v>2002</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>11543100000000</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>51193</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>138000000</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>1342000</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>287600000</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="2">
         <v>4021726</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="3">
         <v>2416425</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <v>16858700000000</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="2">
         <v>106391985300</v>
       </c>
     </row>
@@ -1312,31 +1305,31 @@
       <c r="A35" s="2">
         <v>2003</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>11836430000000</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>51181</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>139400000</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>1431000</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>290100000</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="2">
         <v>4089950</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="3">
         <v>2443387</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="2">
         <v>17533300000000</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="2">
         <v>106687896600</v>
       </c>
     </row>
@@ -1344,31 +1337,31 @@
       <c r="A36" s="2">
         <v>2004</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>12246930000000</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>51109</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>140900000</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>1385000</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>292800000</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="2">
         <v>4112052</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="3">
         <v>2448288</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="2">
         <v>18298400000000</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="2">
         <v>108508357500</v>
       </c>
     </row>
@@ -1376,31 +1369,31 @@
       <c r="A37" s="2">
         <v>2005</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>12622950000000</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>52292</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>143400000</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>1375000</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>295500000</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="2">
         <v>4138349</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="3">
         <v>2397615</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="2">
         <v>19139900000000</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="2">
         <v>108705755300</v>
       </c>
     </row>
@@ -1408,31 +1401,31 @@
       <c r="A38" s="2">
         <v>2006</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>12958480000000</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>53620</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>146000000</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>1414000</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>298400000</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="2">
         <v>4265555</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="3">
         <v>2448017</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <v>19972800000000</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="2">
         <v>108223082400</v>
       </c>
     </row>
@@ -1440,31 +1433,31 @@
       <c r="A39" s="2">
         <v>2007</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>13206380000000</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>53434</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>147600000</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>1413000</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>301200000</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="2">
         <v>4316233</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="3">
         <v>2426264</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <v>20705300000000</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="2">
         <v>110168847900</v>
       </c>
     </row>
@@ -1472,31 +1465,31 @@
       <c r="A40" s="2">
         <v>2008</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>13161930000000</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>51503</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>147000000</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>1498000</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>304100000</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="2">
         <v>4247694</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="3">
         <v>2423712</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="2">
         <v>21234600000000</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="2">
         <v>107871770000</v>
       </c>
     </row>
@@ -1504,31 +1497,31 @@
       <c r="A41" s="2">
         <v>2009</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>12703130000000</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>50410</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>141500000</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>1528000</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>306800000</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="2">
         <v>4130665</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="3">
         <v>2471984</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="2">
         <v>21354500000000</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="2">
         <v>103272113700</v>
       </c>
     </row>
@@ -1536,31 +1529,31 @@
       <c r="A42" s="2">
         <v>2010</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>13087980000000</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>49692</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>140700000</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>1558000</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>309300000</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="2">
         <v>3999386</v>
       </c>
-      <c r="H42" s="6">
+      <c r="H42" s="3">
         <v>2437163</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="2">
         <v>21508000000000</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="2">
         <v>107139605300</v>
       </c>
     </row>
@@ -1568,36 +1561,33 @@
       <c r="A43" s="2">
         <v>2011</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>13315080000000</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>50124</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>141500000</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>1588000</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>311600000</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="2">
         <v>3953593</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H43" s="2">
         <v>2468435</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <v>21763500000000</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="2">
         <v>106735322000</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="H44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Now including .0 at the end of all data to force R to interpret the information as real numbers instead of integers. Was getting an integer overflow from the data when R was importing integers.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -85,6 +85,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,7 +149,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,7 +157,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -468,7 +474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:J43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -569,31 +577,31 @@
       <c r="A12" s="2">
         <v>1980</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>5833975000000</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>39086</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>101400000</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>660939</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>227200000</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>3612258</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>1913841</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <v>7353330000000</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <v>83112760950</v>
       </c>
     </row>
@@ -601,31 +609,31 @@
       <c r="A13" s="2">
         <v>1981</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>5982075000000</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>39099</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>102500000</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>683300</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>229500000</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="3">
         <v>3629238</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>1989841</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <v>7590120000000</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="3">
         <v>81176408930</v>
       </c>
     </row>
@@ -633,31 +641,31 @@
       <c r="A14" s="2">
         <v>1982</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>5865925000000</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>39125</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>101700000</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>711900</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>231700000</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="3">
         <v>3680537</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>1977981</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
         <v>7758610000000</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="3">
         <v>78029441540</v>
       </c>
     </row>
@@ -665,31 +673,31 @@
       <c r="A15" s="2">
         <v>1983</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>6130925000000</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>39871</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>103000000</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>751700</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>233800000</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>3638933</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>1974797</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="3">
         <v>7963160000000</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="3">
         <v>77589648230</v>
       </c>
     </row>
@@ -697,31 +705,31 @@
       <c r="A16" s="2">
         <v>1984</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>6571525000000</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>40421</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>107200000</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>797800</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>235800000</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>3669141</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>2019201</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3">
         <v>8274440000000</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="3">
         <v>81427503780</v>
       </c>
     </row>
@@ -729,31 +737,31 @@
       <c r="A17" s="2">
         <v>1985</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>6843400000000</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>41317</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <v>109400000</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>801900</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>237900000</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>3760561</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>2039369</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="3">
         <v>8616340000000</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="3">
         <v>81355952930</v>
       </c>
     </row>
@@ -761,31 +769,31 @@
       <c r="A18" s="2">
         <v>1986</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>7080500000000</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>42421</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>111800000</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>840381</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>240100000</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>3756547</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>2086440</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="3">
         <v>8950460000000</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="3">
         <v>81578376750</v>
       </c>
     </row>
@@ -793,31 +801,31 @@
       <c r="A19" s="2">
         <v>1987</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>7307050000000</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>42911</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="3">
         <v>114700000</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>895739</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>242300000</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <v>3809394</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>2105361</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="3">
         <v>9271200000000</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="3">
         <v>84205348020</v>
       </c>
     </row>
@@ -825,31 +833,31 @@
       <c r="A20" s="2">
         <v>1988</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>7607400000000</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>43349</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>117200000</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>900195</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>244500000</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>3909510</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>2123323</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3">
         <v>9599010000000</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="3">
         <v>87997172270</v>
       </c>
     </row>
@@ -857,31 +865,31 @@
       <c r="A21" s="2">
         <v>1989</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>7879175000000</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>44081</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
         <v>119600000</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>943036</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>246800000</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <v>4040958</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>2167999</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="3">
         <v>9935250000000</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="3">
         <v>90695352450</v>
       </c>
     </row>
@@ -889,31 +897,31 @@
       <c r="A22" s="2">
         <v>1990</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>8027025000000</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>43344</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>121000000</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>960009</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>249600000</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>4158212</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>2150466</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3">
         <v>10241300000000</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="3">
         <v>91178022420</v>
       </c>
     </row>
@@ -921,31 +929,31 @@
       <c r="A23" s="2">
         <v>1991</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="3">
         <v>8008325000000</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>42726</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="3">
         <v>119800000</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>981659</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>253000000</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>4110907</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>2148463</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
         <v>10475400000000</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="3">
         <v>91154424090</v>
       </c>
     </row>
@@ -953,31 +961,31 @@
       <c r="A24" s="2">
         <v>1992</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>8280025000000</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>43054</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="3">
         <v>120500000</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>1020000</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>256500000</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="3">
         <v>4065014</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>2169518</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
         <v>10744600000000</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="3">
         <v>92448155690</v>
       </c>
     </row>
@@ -985,31 +993,31 @@
       <c r="A25" s="2">
         <v>1993</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>8516175000000</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>44742</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <v>122100000</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>1014000</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>259900000</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>4000240</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>2175613</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
         <v>11065300000000</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="3">
         <v>94232721890</v>
       </c>
     </row>
@@ -1017,31 +1025,31 @@
       <c r="A26" s="2">
         <v>1994</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="3">
         <v>8863125000000</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>45380</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="3">
         <v>124800000</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>1080000</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>263100000</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>3952767</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>2268553</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
         <v>11449300000000</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="3">
         <v>96065748930</v>
       </c>
     </row>
@@ -1049,31 +1057,31 @@
       <c r="A27" s="2">
         <v>1995</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>9085975000000</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>45859</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
         <v>126500000</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <v>1036000</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="3">
         <v>266300000</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="3">
         <v>3899589</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>2278994</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <v>11879000000000</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="3">
         <v>98186495330</v>
       </c>
     </row>
@@ -1081,31 +1089,31 @@
       <c r="A28" s="2">
         <v>1996</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="3">
         <v>9425850000000</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>46823</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <v>128300000</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="3">
         <v>1139000</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="3">
         <v>269400000</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="3">
         <v>3891494</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>2312132</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
         <v>12389100000000</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="3">
         <v>101378213900</v>
       </c>
     </row>
@@ -1113,31 +1121,31 @@
       <c r="A29" s="2">
         <v>1997</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="3">
         <v>9845925000000</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>47995</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <v>131100000</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>1160000</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>272700000</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="3">
         <v>3880894</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="4">
         <v>2314690</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <v>12987200000000</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="3">
         <v>102230767700</v>
       </c>
     </row>
@@ -1145,31 +1153,31 @@
       <c r="A30" s="2">
         <v>1998</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="3">
         <v>10274750000000</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>49276</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="3">
         <v>133000000</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>1199000</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="3">
         <v>275900000</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="3">
         <v>3941553</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="4">
         <v>2314245</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
         <v>13702500000000</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="3">
         <v>102919340800</v>
       </c>
     </row>
@@ -1177,31 +1185,31 @@
       <c r="A31" s="2">
         <v>1999</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="3">
         <v>10770630000000</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>51136</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="3">
         <v>134900000</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>1261000</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>279000000</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="3">
         <v>3959417</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="4">
         <v>2337256</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
         <v>14518800000000</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="3">
         <v>104583817300</v>
       </c>
     </row>
@@ -1209,31 +1217,31 @@
       <c r="A32" s="2">
         <v>2000</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="3">
         <v>11216430000000</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>51388</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <v>138300000</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="3">
         <v>1294000</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>282200000</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="3">
         <v>4058814</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="4">
         <v>2391399</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="3">
         <v>15409200000000</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="3">
         <v>106936290200</v>
       </c>
     </row>
@@ -1241,31 +1249,31 @@
       <c r="A33" s="2">
         <v>2001</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="3">
         <v>11337480000000</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>51478</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>138400000</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>1320000</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>285000000</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="3">
         <v>4025933</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="4">
         <v>2403351</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="3">
         <v>16201300000000</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="3">
         <v>104444769100</v>
       </c>
     </row>
@@ -1273,31 +1281,31 @@
       <c r="A34" s="2">
         <v>2002</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="3">
         <v>11543100000000</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>51193</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="3">
         <v>138000000</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="3">
         <v>1342000</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
         <v>287600000</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="3">
         <v>4021726</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="4">
         <v>2416425</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="3">
         <v>16858700000000</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="3">
         <v>106391985300</v>
       </c>
     </row>
@@ -1305,31 +1313,31 @@
       <c r="A35" s="2">
         <v>2003</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="3">
         <v>11836430000000</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>51181</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <v>139400000</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <v>1431000</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
         <v>290100000</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="3">
         <v>4089950</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="4">
         <v>2443387</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="3">
         <v>17533300000000</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="3">
         <v>106687896600</v>
       </c>
     </row>
@@ -1337,31 +1345,31 @@
       <c r="A36" s="2">
         <v>2004</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="3">
         <v>12246930000000</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>51109</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="3">
         <v>140900000</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="3">
         <v>1385000</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="3">
         <v>292800000</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="3">
         <v>4112052</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="4">
         <v>2448288</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="3">
         <v>18298400000000</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="3">
         <v>108508357500</v>
       </c>
     </row>
@@ -1369,31 +1377,31 @@
       <c r="A37" s="2">
         <v>2005</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="3">
         <v>12622950000000</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <v>52292</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="3">
         <v>143400000</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="3">
         <v>1375000</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="3">
         <v>295500000</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="3">
         <v>4138349</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="4">
         <v>2397615</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="3">
         <v>19139900000000</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="3">
         <v>108705755300</v>
       </c>
     </row>
@@ -1401,31 +1409,31 @@
       <c r="A38" s="2">
         <v>2006</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="3">
         <v>12958480000000</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>53620</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="3">
         <v>146000000</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="3">
         <v>1414000</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="3">
         <v>298400000</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="3">
         <v>4265555</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="4">
         <v>2448017</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="3">
         <v>19972800000000</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="3">
         <v>108223082400</v>
       </c>
     </row>
@@ -1433,31 +1441,31 @@
       <c r="A39" s="2">
         <v>2007</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="3">
         <v>13206380000000</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <v>53434</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="3">
         <v>147600000</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="3">
         <v>1413000</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="3">
         <v>301200000</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="3">
         <v>4316233</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="4">
         <v>2426264</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="3">
         <v>20705300000000</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="3">
         <v>110168847900</v>
       </c>
     </row>
@@ -1465,31 +1473,31 @@
       <c r="A40" s="2">
         <v>2008</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="3">
         <v>13161930000000</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="3">
         <v>51503</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="3">
         <v>147000000</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="3">
         <v>1498000</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="3">
         <v>304100000</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="3">
         <v>4247694</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="4">
         <v>2423712</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="3">
         <v>21234600000000</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="3">
         <v>107871770000</v>
       </c>
     </row>
@@ -1497,31 +1505,31 @@
       <c r="A41" s="2">
         <v>2009</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="3">
         <v>12703130000000</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="3">
         <v>50410</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="3">
         <v>141500000</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="3">
         <v>1528000</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="3">
         <v>306800000</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="3">
         <v>4130665</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="4">
         <v>2471984</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="3">
         <v>21354500000000</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="3">
         <v>103272113700</v>
       </c>
     </row>
@@ -1529,31 +1537,31 @@
       <c r="A42" s="2">
         <v>2010</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="3">
         <v>13087980000000</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="3">
         <v>49692</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="3">
         <v>140700000</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="3">
         <v>1558000</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="3">
         <v>309300000</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="3">
         <v>3999386</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="4">
         <v>2437163</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="3">
         <v>21508000000000</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="3">
         <v>107139605300</v>
       </c>
     </row>
@@ -1561,31 +1569,31 @@
       <c r="A43" s="2">
         <v>2011</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="3">
         <v>13315080000000</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="3">
         <v>50124</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="3">
         <v>141500000</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="3">
         <v>1588000</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="3">
         <v>311600000</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="3">
         <v>3953593</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>2468435</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="3">
         <v>21763500000000</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="3">
         <v>106735322000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited notes correcting units on wage. Wage is actually in $/worker, not $/capita.
</commit_message>
<xml_diff>
--- a/data/USData.xlsx
+++ b/data/USData.xlsx
@@ -69,16 +69,16 @@
     <t>E</t>
   </si>
   <si>
-    <t>w_capita</t>
-  </si>
-  <si>
-    <t># w_capita = Average U.S. wage [2005$/year-capita]</t>
-  </si>
-  <si>
     <t># L =total U.S. labor [workers/year]</t>
   </si>
   <si>
     <t># L_A = number of U.S. researchers in the STEM disciplines [workers/year]</t>
+  </si>
+  <si>
+    <t>w_worker</t>
+  </si>
+  <si>
+    <t># w_worker = Average U.S. wage [2005$/year-worker]</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:J43"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -498,17 +498,17 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -549,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>

</xml_diff>